<commit_message>
Create videos for 'celebrities' topic
</commit_message>
<xml_diff>
--- a/celebrities/celebrities.xlsx
+++ b/celebrities/celebrities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44739\Desktop\The World Blueprint\fact vs fiction\celebrities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F8BCAE-17D6-459E-B96A-A151E7D2136C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EDAF18-2D75-4BCE-9467-507EBD1571A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CC8EF966-1A08-4E05-A262-6FD8005B1731}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
   <si>
     <t>Subject</t>
   </si>
@@ -581,9 +581,6 @@
     <t>Beyoncé’s full name is Beyoncé Carter.</t>
   </si>
   <si>
-    <t>Fact! She holds 32 Grammy Awards.</t>
-  </si>
-  <si>
     <t>Fact! It is said that himself and Amy Wadge wrote the entire thing in his kitchen in 20 minutes.</t>
   </si>
   <si>
@@ -675,6 +672,12 @@
   </si>
   <si>
     <t>Sheeran has acted in Game of Thrones.</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Fact! She holds 35 Grammy Awards.</t>
   </si>
 </sst>
 </file>
@@ -718,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -731,6 +734,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,6 +753,1293 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{703E6D36-7397-EEB5-38B9-2A94167200B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="9326880"/>
+          <a:ext cx="2095500" cy="2800350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>73660</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>71120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D0D9CF7-DC10-8EE3-0E0D-03AF99A22A05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="8961120"/>
+          <a:ext cx="2794000" cy="3911600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>135255</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D836395-BB33-F770-2DC5-7ECAFD3F8D3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="8595360"/>
+          <a:ext cx="2095500" cy="2695575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>73660</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>55880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C8953A3-1475-446A-6072-E23244EA3FDF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="8229600"/>
+          <a:ext cx="2794000" cy="3530600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>670560</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>216408</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{122ACF9D-F4AB-919B-04AF-2F1647CF797F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="7863840"/>
+          <a:ext cx="670560" cy="947928"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AA4206F-C96E-ED2B-2645-A000B0C862AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="7498080"/>
+          <a:ext cx="2095500" cy="3009900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{004F5362-BE2D-61BA-48C8-416B75F88C97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="7315200"/>
+          <a:ext cx="2095500" cy="2828925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7167256-08B5-00DF-6549-E1AEF41E443E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="7132320"/>
+          <a:ext cx="2095500" cy="3352800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>73660</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26DEBA43-2EDB-C64A-7E2A-E2F5C3860BDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="6766560"/>
+          <a:ext cx="2794000" cy="3606800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>422910</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D62CA11-3788-373A-A166-E944136DC57D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="6583680"/>
+          <a:ext cx="3143250" cy="4533900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>73660</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>17780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F5784BB-027A-B5C3-D564-1E9E9C1EEBA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="6400800"/>
+          <a:ext cx="2794000" cy="3492500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>59055</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B798A53-22EB-41F3-F99E-7B732617A1CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="6035040"/>
+          <a:ext cx="2095500" cy="2619375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>454660</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36F94EB6-42E8-6946-5DE4-CA6014AA2EAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="5669280"/>
+          <a:ext cx="3175000" cy="3683000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>276225</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{766D8526-622C-D13A-5A04-267155884A03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="5486400"/>
+          <a:ext cx="2095500" cy="3019425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>73660</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>337820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AA03151-4C8D-1B6F-1E9B-3030104B0969}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="5120640"/>
+          <a:ext cx="2794000" cy="4178300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3262243C-CBE5-1A73-40D0-E55945BA5F1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="4754880"/>
+          <a:ext cx="2095500" cy="2790825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>73660</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A302B7AD-EC13-AAE0-6072-D6968FBBCCBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="4389120"/>
+          <a:ext cx="2794000" cy="3695700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D78A166B-B16B-77CF-B8DC-B67D23D23073}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="4206240"/>
+          <a:ext cx="2095500" cy="3143250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>40005</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B946D9F3-D5E7-1A02-0A03-2ECA2DAF5E89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="3840480"/>
+          <a:ext cx="2095500" cy="2600325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>74297</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>173635</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ACB3682-851C-113C-6AF3-E5E73D1FF575}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="3474720"/>
+          <a:ext cx="2794637" cy="4014115"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>73660</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>27940</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66E1C758-82BF-4F0E-9FC7-93209B6858E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="3108960"/>
+          <a:ext cx="2794000" cy="4051300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D009750-D605-BF05-C806-6AEC6A3A631F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="2743200"/>
+          <a:ext cx="2095500" cy="3028950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD98D9C5-D5EC-E496-F234-626601873119}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="2377440"/>
+          <a:ext cx="2095500" cy="2743200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D039E5D7-D4F3-1B8D-F0AE-EF146A3C9436}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="2011680"/>
+          <a:ext cx="2095500" cy="2790825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAE13B36-72B7-8890-975C-8C2D6E499C98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="1645920"/>
+          <a:ext cx="2095500" cy="3095625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>362713</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04BC504C-F59D-8ABA-44C2-A714A6F8A22C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="1280160"/>
+          <a:ext cx="609601" cy="728473"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>306705</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15C6E2D4-4264-7850-3B2D-8489EE8B6E70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="914400"/>
+          <a:ext cx="2095500" cy="2867025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>249555</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A80763D9-5F5F-A71B-D8F9-BC4E28A83385}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="548640"/>
+          <a:ext cx="2095500" cy="2809875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>73660</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>187960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4757E9F1-0797-EEA5-D633-CB81AAD29CD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26601420" y="182880"/>
+          <a:ext cx="2794000" cy="3479800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1068,8 +2361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBEE15E8-303E-4237-A1ED-3CA08FA56CCA}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1077,6 +2370,7 @@
     <col min="1" max="1" width="20.77734375" customWidth="1"/>
     <col min="2" max="9" width="40.77734375" customWidth="1"/>
     <col min="10" max="10" width="40.88671875" customWidth="1"/>
+    <col min="11" max="11" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -1087,30 +2381,32 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="K1" s="4"/>
+      <c r="K1" s="5" t="s">
+        <v>212</v>
+      </c>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
@@ -1235,17 +2531,17 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
@@ -1278,7 +2574,7 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>168</v>
@@ -1340,7 +2636,7 @@
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -1365,7 +2661,7 @@
         <v>118</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>119</v>
@@ -1398,7 +2694,7 @@
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -1510,10 +2806,10 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="4"/>
@@ -1644,7 +2940,7 @@
         <v>78</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
@@ -1767,11 +3063,11 @@
         <v>108</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
@@ -1800,7 +3096,7 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
@@ -1815,7 +3111,7 @@
         <v>146</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>147</v>
@@ -1844,10 +3140,10 @@
         <v>152</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
@@ -1858,7 +3154,7 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>155</v>
@@ -1902,11 +3198,11 @@
         <v>163</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>164</v>
@@ -1928,27 +3224,27 @@
     </row>
     <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="4"/>
@@ -1957,5 +3253,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>